<commit_message>
Glowing eyes genes 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/LTS/Glowing eyes genes - 3023336989/3023336989.xlsx
+++ b/Data/LTS/Glowing eyes genes - 3023336989/3023336989.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.6.2\Glowing eyes genes - 3023336989\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\LTS\Glowing eyes genes - 3023336989\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DDED82-C141-4005-B975-440A86545D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA0B753-2AA4-4691-8D11-3712A4089ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240327" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_250630" sheetId="2" r:id="rId1"/>
+    <sheet name="Old_240327" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -179,6 +180,42 @@
   </si>
   <si>
     <t>빛나는 붉은 눈</t>
+  </si>
+  <si>
+    <t>GeneDef+GEG_Eyes_GlowingWhite.label</t>
+  </si>
+  <si>
+    <t>GEG_Eyes_GlowingWhite.label</t>
+  </si>
+  <si>
+    <t>빛나는 백색 눈</t>
+  </si>
+  <si>
+    <t>GeneDef+GEG_Eyes_GlowingWhite.description</t>
+  </si>
+  <si>
+    <t>GEG_Eyes_GlowingWhite.description</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 홍채에 생물발광성 순백색 색소를 가지고 있습니다.</t>
+  </si>
+  <si>
+    <t>GeneDef+GEG_Eyes_GlowingNoctol.label</t>
+  </si>
+  <si>
+    <t>GEG_Eyes_GlowingNoctol.label</t>
+  </si>
+  <si>
+    <t>빛나는 암귀 눈</t>
+  </si>
+  <si>
+    <t>GeneDef+GEG_Eyes_GlowingNoctol.description</t>
+  </si>
+  <si>
+    <t>GEG_Eyes_GlowingNoctol.description</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 홍채에 생물발광성 '암귀의 노란색' 색소를 가지고 있습니다.</t>
   </si>
 </sst>
 </file>
@@ -563,25 +600,266 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D747698-8C9B-49A1-BD2D-FE3A17CCE595}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="49.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -616,7 +894,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -631,7 +909,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -648,7 +926,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -665,7 +943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -682,7 +960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -699,7 +977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -716,7 +994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -733,7 +1011,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -750,7 +1028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -767,7 +1045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -784,7 +1062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>

</xml_diff>